<commit_message>
changes to obstacle doc
</commit_message>
<xml_diff>
--- a/Documents/Obsticle positioning.xlsx
+++ b/Documents/Obsticle positioning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s191265\Documents\MeanBeanStudio\MeanBeanStudio\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066B0F98-2652-470F-86F6-D2FF21F8DD94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80F68FD-F034-498F-99A5-9508E54144FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C1565F42-A131-4FF6-90EF-ACB1D2A58EC7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Left</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">risks/ may cause problems </t>
   </si>
 </sst>
 </file>
@@ -607,7 +610,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,6 +703,10 @@
       <c r="E5" s="7"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
+      <c r="J5" s="20"/>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>